<commit_message>
quantlib | python final
</commit_message>
<xml_diff>
--- a/Python/QuantLibStuff/FinalQuantLibSub/instruments.xlsx
+++ b/Python/QuantLibStuff/FinalQuantLibSub/instruments.xlsx
@@ -476,10 +476,10 @@
         <v>0.025</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03206338030688434</v>
+        <v>0.03205053372796332</v>
       </c>
       <c r="E2" t="n">
-        <v>-342255.781872031</v>
+        <v>-342529.9652282526</v>
       </c>
     </row>
     <row r="3">
@@ -603,10 +603,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.02510157848820124</v>
+        <v>0.02508731863097187</v>
       </c>
       <c r="E2" t="n">
-        <v>128296.956717473</v>
+        <v>128224.0730027451</v>
       </c>
     </row>
     <row r="3">
@@ -624,10 +624,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.03573138314070221</v>
+        <v>0.03570358392086448</v>
       </c>
       <c r="E3" t="n">
-        <v>180641.9925446612</v>
+        <v>180501.4520443704</v>
       </c>
     </row>
     <row r="4">
@@ -645,10 +645,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.03296290464331172</v>
+        <v>0.0329919142530939</v>
       </c>
       <c r="E4" t="n">
-        <v>168477.0681769266</v>
+        <v>168625.3395158133</v>
       </c>
     </row>
     <row r="5">
@@ -666,10 +666,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.03165657792135292</v>
+        <v>0.03161977715018041</v>
       </c>
       <c r="E5" t="n">
-        <v>159162.2389934688</v>
+        <v>158977.2128939626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>